<commit_message>
Save plots for multi p
</commit_message>
<xml_diff>
--- a/Part 1/Runs/Part1b/Pie_plots_multiple_channels/Multiple_Channels.xlsx
+++ b/Part 1/Runs/Part1b/Pie_plots_multiple_channels/Multiple_Channels.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1ABC38-0054-471B-B216-C010197AB013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="1050" windowWidth="23025" windowHeight="10350" tabRatio="831" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4980" yWindow="1050" windowWidth="23025" windowHeight="10350" tabRatio="831"/>
   </bookViews>
   <sheets>
     <sheet name="Run_1_Chanells_2_BER_0.01" sheetId="2" r:id="rId1"/>
@@ -23,13 +23,41 @@
     <sheet name="Run_8_Chanells_10_BER_0.01" sheetId="9" r:id="rId8"/>
     <sheet name="Run_9_Chanells_10_BER_0.01" sheetId="10" r:id="rId9"/>
     <sheet name="Run_10_Chanells_10_BER_0.01" sheetId="11" r:id="rId10"/>
+    <sheet name="Run_11_Chanells_10_BER_0.01" sheetId="12" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>dmin</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Data_Portion</t>
+  </si>
+  <si>
+    <t>Bitrate</t>
+  </si>
+  <si>
+    <t>BER with ECC</t>
+  </si>
   <si>
     <t>Channel</t>
   </si>
@@ -322,7 +350,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -330,34 +358,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
@@ -674,24 +704,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="3" bestFit="true" customWidth="true"/>
+    <col min="2" max="3" width="4.5703125" style="3" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="6.28515625" style="4" customWidth="true"/>
+    <col min="5" max="5" width="5.5703125" style="3" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="4.5703125" style="2" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="12.5703125" style="4" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="9.5703125" style="5" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="12.42578125" style="5" bestFit="true" customWidth="true"/>
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -720,7 +750,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -749,7 +779,7 @@
         <v>3.0993801239752048E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -794,18 +824,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="2" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="2.140625" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="6.28515625" customWidth="true"/>
+    <col min="5" max="5" width="5.5703125" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="12" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="12.5703125" style="1" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="12" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="12.42578125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>81</v>
       </c>
@@ -834,7 +864,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -863,7 +893,7 @@
         <v>3.5992801439712059E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -892,7 +922,7 @@
         <v>3.4993001399720057E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -921,7 +951,7 @@
         <v>2.1995600879824036E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -950,7 +980,7 @@
         <v>3.2993401319736052E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -979,7 +1009,7 @@
         <v>3.6985205917632949E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1008,7 +1038,7 @@
         <v>1.8992403038784486E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1037,7 +1067,7 @@
         <v>6.2968515742128934E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1066,7 +1096,7 @@
         <v>4.197901049475262E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1095,7 +1125,7 @@
         <v>3.8992201559688061E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1126,6 +1156,345 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I11"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" customWidth="true"/>
+    <col min="2" max="2" width="2.140625" customWidth="true"/>
+    <col min="3" max="3" width="2.28515625" customWidth="true"/>
+    <col min="4" max="4" width="14.7109375" customWidth="true"/>
+    <col min="5" max="5" width="5.7109375" customWidth="true"/>
+    <col min="6" max="6" width="12.7109375" customWidth="true"/>
+    <col min="7" max="7" width="13.7109375" customWidth="true"/>
+    <col min="8" max="8" width="11.7109375" customWidth="true"/>
+    <col min="9" max="9" width="14.7109375" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0">
+        <v>3</v>
+      </c>
+      <c r="D2" s="0">
+        <v>0.002</v>
+      </c>
+      <c r="E2" s="0">
+        <v>2</v>
+      </c>
+      <c r="F2" s="0">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G2" s="0">
+        <v>0.16055045871559631</v>
+      </c>
+      <c r="H2" s="0">
+        <v>666666.66666666663</v>
+      </c>
+      <c r="I2" s="0">
+        <v>0.0028994201159768048</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0">
+        <v>5</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0.0073333333333333332</v>
+      </c>
+      <c r="E3" s="0">
+        <v>3</v>
+      </c>
+      <c r="F3" s="0">
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="G3" s="0">
+        <v>0.096330275229357804</v>
+      </c>
+      <c r="H3" s="0">
+        <v>400000</v>
+      </c>
+      <c r="I3" s="0">
+        <v>0.00019996000799840031</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0">
+        <v>2</v>
+      </c>
+      <c r="C4" s="0">
+        <v>5</v>
+      </c>
+      <c r="D4" s="0">
+        <v>0.012666666666666666</v>
+      </c>
+      <c r="E4" s="0">
+        <v>3</v>
+      </c>
+      <c r="F4" s="0">
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="G4" s="0">
+        <v>0.096330275229357804</v>
+      </c>
+      <c r="H4" s="0">
+        <v>400000</v>
+      </c>
+      <c r="I4" s="0">
+        <v>0.00099980003999200159</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0">
+        <v>2</v>
+      </c>
+      <c r="C5" s="0">
+        <v>5</v>
+      </c>
+      <c r="D5" s="0">
+        <v>0.018000000000000002</v>
+      </c>
+      <c r="E5" s="0">
+        <v>3</v>
+      </c>
+      <c r="F5" s="0">
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="G5" s="0">
+        <v>0.096330275229357804</v>
+      </c>
+      <c r="H5" s="0">
+        <v>400000</v>
+      </c>
+      <c r="I5" s="0">
+        <v>0.0010997800439912018</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0">
+        <v>5</v>
+      </c>
+      <c r="D6" s="0">
+        <v>0.023333333333333331</v>
+      </c>
+      <c r="E6" s="0">
+        <v>3</v>
+      </c>
+      <c r="F6" s="0">
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="G6" s="0">
+        <v>0.096330275229357804</v>
+      </c>
+      <c r="H6" s="0">
+        <v>400000</v>
+      </c>
+      <c r="I6" s="0">
+        <v>0.0035992801439712059</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0">
+        <v>2</v>
+      </c>
+      <c r="C7" s="0">
+        <v>5</v>
+      </c>
+      <c r="D7" s="0">
+        <v>0.028666666666666667</v>
+      </c>
+      <c r="E7" s="0">
+        <v>3</v>
+      </c>
+      <c r="F7" s="0">
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="G7" s="0">
+        <v>0.096330275229357804</v>
+      </c>
+      <c r="H7" s="0">
+        <v>400000</v>
+      </c>
+      <c r="I7" s="0">
+        <v>0.0043991201759648072</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0">
+        <v>2</v>
+      </c>
+      <c r="C8" s="0">
+        <v>5</v>
+      </c>
+      <c r="D8" s="0">
+        <v>0.034000000000000002</v>
+      </c>
+      <c r="E8" s="0">
+        <v>3</v>
+      </c>
+      <c r="F8" s="0">
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="G8" s="0">
+        <v>0.096330275229357804</v>
+      </c>
+      <c r="H8" s="0">
+        <v>400000</v>
+      </c>
+      <c r="I8" s="0">
+        <v>0.0054989002199560084</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0">
+        <v>5</v>
+      </c>
+      <c r="D9" s="0">
+        <v>0.039333333333333338</v>
+      </c>
+      <c r="E9" s="0">
+        <v>3</v>
+      </c>
+      <c r="F9" s="0">
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="G9" s="0">
+        <v>0.096330275229357804</v>
+      </c>
+      <c r="H9" s="0">
+        <v>400000</v>
+      </c>
+      <c r="I9" s="0">
+        <v>0.0072985402919416116</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0">
+        <v>2</v>
+      </c>
+      <c r="C10" s="0">
+        <v>5</v>
+      </c>
+      <c r="D10" s="0">
+        <v>0.044666666666666667</v>
+      </c>
+      <c r="E10" s="0">
+        <v>3</v>
+      </c>
+      <c r="F10" s="0">
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="G10" s="0">
+        <v>0.096330275229357804</v>
+      </c>
+      <c r="H10" s="0">
+        <v>400000</v>
+      </c>
+      <c r="I10" s="0">
+        <v>0.0099980003999200154</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0">
+        <v>2</v>
+      </c>
+      <c r="C11" s="0">
+        <v>7</v>
+      </c>
+      <c r="D11" s="0">
+        <v>0.050000000000000003</v>
+      </c>
+      <c r="E11" s="0">
+        <v>4</v>
+      </c>
+      <c r="F11" s="0">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="G11" s="0">
+        <v>0.068807339449541274</v>
+      </c>
+      <c r="H11" s="0">
+        <v>285714.28571428568</v>
+      </c>
+      <c r="I11" s="0">
+        <v>0.009398120375924815</v>
+      </c>
+    </row>
+  </sheetData>
 </worksheet>
 </file>
 
@@ -1139,19 +1508,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" style="6" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="2" style="6" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="3" style="6" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="6.28515625" style="4" customWidth="true"/>
+    <col min="5" max="5" width="5.5703125" style="3" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="12" style="7" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="12.5703125" style="8" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="12" style="5" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="12.42578125" style="5" bestFit="true" customWidth="true"/>
     <col min="10" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -1180,7 +1549,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1209,7 +1578,7 @@
         <v>1.8999962000076E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1238,49 +1607,49 @@
         <v>5.6999886000227999E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="F4" s="2"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="F5" s="2"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="F6" s="2"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="F7" s="2"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="F8" s="2"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="F9" s="2"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1302,18 +1671,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="2" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="3" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="6.28515625" customWidth="true"/>
+    <col min="5" max="5" width="5.5703125" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="12" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="12.5703125" style="1" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="12" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="12.42578125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -1342,7 +1711,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1371,7 +1740,7 @@
         <v>3.7981009495252375E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1400,7 +1769,7 @@
         <v>5.0974512743628183E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1411,7 +1780,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1422,7 +1791,7 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1433,7 +1802,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1444,7 +1813,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1455,7 +1824,7 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1466,7 +1835,7 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1492,18 +1861,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="2" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="2.140625" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="6.28515625" customWidth="true"/>
+    <col min="5" max="5" width="5.5703125" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="12" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="12.5703125" style="1" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="12" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="12.42578125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -1532,7 +1901,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1561,7 +1930,7 @@
         <v>2.3995200959808036E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1590,7 +1959,7 @@
         <v>3.199360127974405E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1619,7 +1988,7 @@
         <v>1.299740051989602E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1648,7 +2017,7 @@
         <v>2.0995800839832034E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1677,7 +2046,7 @@
         <v>2.3995200959808036E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1706,7 +2075,7 @@
         <v>4.0991801639672061E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1735,7 +2104,7 @@
         <v>6.4987002599480106E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1764,7 +2133,7 @@
         <v>8.0983803239352125E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1793,7 +2162,7 @@
         <v>9.4981003799240148E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1837,18 +2206,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="2" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="3" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="6.28515625" customWidth="true"/>
+    <col min="5" max="5" width="5.5703125" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="12" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="12.5703125" style="1" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="12" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="12.42578125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -1877,7 +2246,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1906,7 +2275,7 @@
         <v>3.9999200015999681E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1935,7 +2304,7 @@
         <v>2.9999400011999759E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1964,7 +2333,7 @@
         <v>8.0998380032399351E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1993,7 +2362,7 @@
         <v>4.4999100017999638E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2022,7 +2391,7 @@
         <v>2.5999480010399791E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2051,7 +2420,7 @@
         <v>3.899922001559969E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2080,7 +2449,7 @@
         <v>6.6998660026799462E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2109,7 +2478,7 @@
         <v>9.0998180036399277E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2138,7 +2507,7 @@
         <v>5.5998880022399555E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2182,18 +2551,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="2" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="3" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="6.28515625" customWidth="true"/>
+    <col min="5" max="5" width="5.5703125" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="12" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="12.5703125" style="1" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="12" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="12.42578125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>45</v>
       </c>
@@ -2222,7 +2591,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2251,7 +2620,7 @@
         <v>2.3999952000095999E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2280,7 +2649,7 @@
         <v>7.7999844000312005E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2309,7 +2678,7 @@
         <v>3.3999932000136E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2338,7 +2707,7 @@
         <v>3.2999934000131997E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2367,7 +2736,7 @@
         <v>8.7999824000351996E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2396,7 +2765,7 @@
         <v>3.9999920000159999E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2425,7 +2794,7 @@
         <v>6.4999870000260004E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2454,7 +2823,7 @@
         <v>4.2999914000172002E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2483,7 +2852,7 @@
         <v>4.8999902000196E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2527,17 +2896,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="true" customWidth="true"/>
+    <col min="2" max="3" width="3" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="6.28515625" customWidth="true"/>
+    <col min="5" max="5" width="5.5703125" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="12" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="12.5703125" style="1" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="12" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="12.42578125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>54</v>
       </c>
@@ -2566,7 +2935,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2595,7 +2964,7 @@
         <v>3.6992601479704061E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2624,7 +2993,7 @@
         <v>7.796881247501E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2653,7 +3022,7 @@
         <v>9.3953023488255877E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2682,7 +3051,7 @@
         <v>3.199360127974405E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2711,7 +3080,7 @@
         <v>6.5980205938218532E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2740,7 +3109,7 @@
         <v>8.193445243804956E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2769,7 +3138,7 @@
         <v>5.0959232613908877E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2798,7 +3167,7 @@
         <v>9.6903096903096907E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2827,7 +3196,7 @@
         <v>8.8911088911088915E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2871,18 +3240,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="2" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="3" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="6.28515625" customWidth="true"/>
+    <col min="5" max="5" width="5.5703125" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="12" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="12.5703125" style="1" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="12" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="12.42578125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>63</v>
       </c>
@@ -2911,7 +3280,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2940,7 +3309,7 @@
         <v>2.7994401119776045E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2969,7 +3338,7 @@
         <v>4.0991801639672061E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2998,7 +3367,7 @@
         <v>6.9986002799440113E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3027,7 +3396,7 @@
         <v>2.2995400919816038E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3056,7 +3425,7 @@
         <v>4.9980007996801284E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -3085,7 +3454,7 @@
         <v>6.6973210715713712E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -3114,7 +3483,7 @@
         <v>9.7951024487756121E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3143,7 +3512,7 @@
         <v>8.6956521739130436E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3172,7 +3541,7 @@
         <v>5.0989802039592084E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -3216,18 +3585,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="2" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="3" bestFit="true" customWidth="true"/>
+    <col min="4" max="4" width="6.28515625" customWidth="true"/>
+    <col min="5" max="5" width="5.5703125" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="12" bestFit="true" customWidth="true"/>
+    <col min="7" max="7" width="12.5703125" style="1" bestFit="true" customWidth="true"/>
+    <col min="8" max="8" width="12" bestFit="true" customWidth="true"/>
+    <col min="9" max="9" width="12.42578125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>72</v>
       </c>
@@ -3256,7 +3625,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3285,7 +3654,7 @@
         <v>4.6990601879624075E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3314,7 +3683,7 @@
         <v>7.8984203159368129E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3343,7 +3712,7 @@
         <v>3.9992001599680062E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3372,7 +3741,7 @@
         <v>1.9996000799840031E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3401,7 +3770,7 @@
         <v>1.1995201919232307E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -3430,7 +3799,7 @@
         <v>1.7992802878848461E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -3459,7 +3828,7 @@
         <v>9.2953523238380811E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3488,7 +3857,7 @@
         <v>6.6966516741629187E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3517,7 +3886,7 @@
         <v>3.9992001599680062E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>

</xml_diff>